<commit_message>
fix circle-block p style
</commit_message>
<xml_diff>
--- a/残作業リスト.xlsx
+++ b/残作業リスト.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12330" activeTab="3"/>
+    <workbookView windowWidth="28125" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="日本" sheetId="2" r:id="rId1"/>
@@ -576,9 +576,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_-&quot;\&quot;* #,##0.00_-\ ;\-&quot;\&quot;* #,##0.00_-\ ;_-&quot;\&quot;* &quot;-&quot;??_-\ ;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-&quot;\&quot;* #,##0_-\ ;\-&quot;\&quot;* #,##0_-\ ;_-&quot;\&quot;* &quot;-&quot;??_-\ ;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;\&quot;* #,##0.00_-\ ;\-&quot;\&quot;* #,##0.00_-\ ;_-&quot;\&quot;* &quot;-&quot;??_-\ ;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -612,14 +612,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="游ゴシック"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="游ゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -639,6 +632,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="游ゴシック"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -650,21 +650,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="游ゴシック"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="游ゴシック"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="游ゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -726,15 +711,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFFFFFF"/>
       <name val="游ゴシック"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="游ゴシック"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="游ゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -745,6 +737,14 @@
       <color theme="1"/>
       <name val="游ゴシック"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="游ゴシック"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -813,6 +813,156 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -825,97 +975,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -927,67 +987,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1092,15 +1092,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1126,6 +1117,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1134,16 +1134,16 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1155,124 +1155,124 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1969,8 +1969,8 @@
   <sheetPr/>
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="30" customHeight="1" outlineLevelCol="4"/>
@@ -3509,7 +3509,7 @@
   <sheetPr/>
   <dimension ref="D1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
form of word fix by HYP
</commit_message>
<xml_diff>
--- a/残作業リスト.xlsx
+++ b/残作業リスト.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12330"/>
+    <workbookView windowWidth="28125" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="日本" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="152">
   <si>
     <t>No.</t>
   </si>
@@ -311,7 +311,13 @@
 DX推進体制   add border</t>
   </si>
   <si>
+    <t>ok</t>
+  </si>
+  <si>
     <t>採用情報＞新卒/第二新卒募集要項＞職場風景</t>
+  </si>
+  <si>
+    <t>to confirm</t>
   </si>
   <si>
     <t>Cloud Deploy/Migration
@@ -322,9 +328,6 @@
   <si>
     <t>改行しない
 Bold なし</t>
-  </si>
-  <si>
-    <t>ok</t>
   </si>
   <si>
     <t>Space</t>
@@ -576,8 +579,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="_-&quot;\&quot;* #,##0.00_-\ ;\-&quot;\&quot;* #,##0.00_-\ ;_-&quot;\&quot;* &quot;-&quot;??_-\ ;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;\&quot;* #,##0_-\ ;\-&quot;\&quot;* #,##0_-\ ;_-&quot;\&quot;* &quot;-&quot;??_-\ ;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;\&quot;* #,##0_-\ ;\-&quot;\&quot;* #,##0_-\ ;_-&quot;\&quot;* &quot;-&quot;??_-\ ;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;\&quot;* #,##0.00_-\ ;\-&quot;\&quot;* #,##0.00_-\ ;_-&quot;\&quot;* &quot;-&quot;??_-\ ;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
@@ -611,8 +614,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="游ゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -655,6 +659,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="游ゴシック"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="游ゴシック"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="游ゴシック"/>
@@ -686,14 +705,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="游ゴシック"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="游ゴシック"/>
@@ -711,9 +722,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
       <name val="游ゴシック"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -725,26 +736,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="游ゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="游ゴシック"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="游ゴシック"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -768,12 +771,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -783,12 +798,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -813,13 +822,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -831,91 +960,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -933,49 +978,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -987,7 +996,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1029,6 +1038,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1059,15 +1079,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1086,8 +1097,26 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1106,26 +1135,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1134,149 +1143,149 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1286,19 +1295,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
@@ -1313,13 +1325,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1967,13 +1979,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="30" customHeight="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="30" customHeight="1" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="6.33333333333333" customWidth="1"/>
     <col min="2" max="2" width="41.8333333333333" customWidth="1"/>
@@ -1982,998 +1994,1013 @@
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:5">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:5">
-      <c r="A2" s="12">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" ht="46" customHeight="1" spans="1:5">
-      <c r="A3" s="12">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" ht="281.25" spans="1:5">
-      <c r="A4" s="12">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:5">
-      <c r="A5" s="12">
+      <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:5">
-      <c r="A6" s="12">
+      <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" s="5" customFormat="1" ht="101" customHeight="1" spans="1:5">
-      <c r="A7" s="12">
+      <c r="E6" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" s="6" customFormat="1" ht="101" customHeight="1" spans="1:5">
+      <c r="A7" s="13">
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:5">
-      <c r="A8" s="12">
+      <c r="A8" s="13">
         <v>7</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:5">
-      <c r="A9" s="12">
-        <v>8</v>
-      </c>
-      <c r="B9" s="12" t="s">
+      <c r="A9" s="13">
+        <v>8</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:5">
-      <c r="A10" s="12">
+      <c r="A10" s="13">
         <v>9</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" ht="39" customHeight="1" spans="1:5">
-      <c r="A11" s="12">
+      <c r="A11" s="13">
         <v>10</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:5">
-      <c r="A12" s="12">
+      <c r="A12" s="13">
         <v>11</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" ht="91" customHeight="1" spans="1:5">
-      <c r="A13" s="12">
+      <c r="A13" s="13">
         <v>12</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" ht="150" customHeight="1" spans="1:5">
-      <c r="A14" s="12">
+      <c r="A14" s="13">
         <v>13</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12" t="s">
+      <c r="C14" s="13"/>
+      <c r="D14" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" ht="137" customHeight="1" spans="1:5">
-      <c r="A15" s="12">
+      <c r="A15" s="13">
         <v>14</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12" t="s">
+      <c r="C15" s="13"/>
+      <c r="D15" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="1:5">
-      <c r="A16" s="12">
+      <c r="A16" s="13">
         <v>15</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="14" t="s">
+      <c r="C16" s="13"/>
+      <c r="D16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" customHeight="1" spans="1:5">
-      <c r="A17" s="12">
+      <c r="A17" s="13">
         <v>16</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12" t="s">
+      <c r="C17" s="13"/>
+      <c r="D17" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="1:5">
-      <c r="A18" s="12">
+      <c r="A18" s="13">
         <v>17</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" customHeight="1" spans="1:5">
-      <c r="A19" s="12">
+      <c r="A19" s="13">
         <v>18</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="14" t="s">
+      <c r="C19" s="13"/>
+      <c r="D19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" customHeight="1" spans="1:5">
-      <c r="A20" s="12">
+      <c r="A20" s="13">
         <v>19</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" customHeight="1" spans="1:5">
-      <c r="A21" s="12">
+      <c r="A21" s="13">
         <v>20</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" s="11" customFormat="1" ht="54" customHeight="1" spans="1:5">
-      <c r="A22" s="12">
+      <c r="E21" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" s="12" customFormat="1" ht="54" customHeight="1" spans="1:5">
+      <c r="A22" s="13">
         <v>21</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" s="11" customFormat="1" ht="60" customHeight="1" spans="1:5">
-      <c r="A23" s="12">
+      <c r="E22" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" s="12" customFormat="1" ht="60" customHeight="1" spans="1:5">
+      <c r="A23" s="13">
         <v>22</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" s="11" customFormat="1" customHeight="1" spans="1:5">
-      <c r="A24" s="12">
+      <c r="E23" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" s="12" customFormat="1" customHeight="1" spans="1:5">
+      <c r="A24" s="13">
         <v>23</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" s="11" customFormat="1" customHeight="1" spans="1:5">
-      <c r="A25" s="12">
+      <c r="E24" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" s="12" customFormat="1" customHeight="1" spans="1:5">
+      <c r="A25" s="13">
         <v>24</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12" t="s">
+      <c r="C25" s="13"/>
+      <c r="D25" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" s="11" customFormat="1" ht="94" customHeight="1" spans="1:5">
-      <c r="A26" s="12">
+      <c r="E25" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" s="12" customFormat="1" ht="94" customHeight="1" spans="1:5">
+      <c r="A26" s="13">
         <v>25</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" s="11" customFormat="1" customHeight="1" spans="1:5">
-      <c r="A27" s="12">
+      <c r="E26" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" s="12" customFormat="1" customHeight="1" spans="1:5">
+      <c r="A27" s="13">
         <v>26</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" s="11" customFormat="1" customHeight="1" spans="1:5">
-      <c r="A28" s="12">
+      <c r="E27" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" s="12" customFormat="1" customHeight="1" spans="1:5">
+      <c r="A28" s="13">
         <v>27</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="29" customHeight="1" spans="1:5">
-      <c r="A29" s="12">
+      <c r="A29" s="13">
         <v>28</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="30" customHeight="1" spans="1:5">
-      <c r="A30" s="12">
+      <c r="A30" s="13">
         <v>29</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="31" customHeight="1" spans="1:5">
-      <c r="A31" s="12">
+      <c r="A31" s="13">
         <v>30</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="32" customHeight="1" spans="1:5">
-      <c r="A32" s="12">
+      <c r="A32" s="13">
         <v>31</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12" t="s">
+      <c r="C32" s="13"/>
+      <c r="D32" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="33" customHeight="1" spans="1:5">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12" t="s">
+      <c r="C33" s="13"/>
+      <c r="D33" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="34" customHeight="1" spans="1:5">
-      <c r="A34" s="12">
+      <c r="A34" s="13">
         <v>33</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="35" customHeight="1" spans="1:5">
-      <c r="A35" s="12">
+      <c r="A35" s="13">
         <v>34</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E35" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="36" customHeight="1" spans="1:5">
-      <c r="A36" s="12">
+      <c r="A36" s="13">
         <v>35</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12" t="s">
+      <c r="C36" s="13"/>
+      <c r="D36" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="37" customHeight="1" spans="1:5">
-      <c r="A37" s="12">
+      <c r="A37" s="13">
         <v>36</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E37" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="38" customHeight="1" spans="1:5">
-      <c r="A38" s="12">
+      <c r="A38" s="13">
         <v>37</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D38" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E38" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="39" customHeight="1" spans="1:5">
-      <c r="A39" s="12">
+      <c r="A39" s="13">
         <v>38</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12" t="s">
+      <c r="C39" s="13"/>
+      <c r="D39" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="40" customHeight="1" spans="1:5">
-      <c r="A40" s="12">
+      <c r="A40" s="13">
         <v>39</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12" t="s">
+      <c r="C40" s="13"/>
+      <c r="D40" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="41" ht="107" customHeight="1" spans="1:5">
-      <c r="A41" s="8">
+      <c r="A41" s="9">
         <v>40</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E41" s="8"/>
-    </row>
-    <row r="42" customHeight="1" spans="1:5">
-      <c r="A42" s="8">
+      <c r="E41" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" customHeight="1" spans="1:6">
+      <c r="A42" s="9">
         <v>41</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E42" s="9"/>
+      <c r="F42" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" ht="156" customHeight="1" spans="1:5">
+      <c r="A43" s="9">
+        <v>42</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8" t="s">
+    </row>
+    <row r="44" ht="73" customHeight="1" spans="1:5">
+      <c r="A44" s="9">
+        <v>43</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E42" s="8"/>
-    </row>
-    <row r="43" ht="156" customHeight="1" spans="1:5">
-      <c r="A43" s="8">
-        <v>42</v>
-      </c>
-      <c r="B43" s="8" t="s">
+      <c r="E44" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" ht="291" customHeight="1" spans="1:5">
+      <c r="A45" s="9">
+        <v>44</v>
+      </c>
+      <c r="B45" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C43" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D43" s="8" t="s">
+      <c r="C45" s="9"/>
+      <c r="D45" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E43" s="8"/>
-    </row>
-    <row r="44" ht="73" customHeight="1" spans="1:5">
-      <c r="A44" s="8">
-        <v>43</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8" t="s">
+      <c r="E45" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" ht="397" customHeight="1" spans="1:5">
+      <c r="A46" s="9">
+        <v>45</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E44" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" ht="291" customHeight="1" spans="1:5">
-      <c r="A45" s="8">
-        <v>44</v>
-      </c>
-      <c r="B45" s="8" t="s">
+      <c r="E46" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" ht="386" customHeight="1" spans="1:5">
+      <c r="A47" s="9">
+        <v>46</v>
+      </c>
+      <c r="B47" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8" t="s">
+      <c r="C47" s="9"/>
+      <c r="D47" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E45" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="46" ht="397" customHeight="1" spans="1:5">
-      <c r="A46" s="8">
-        <v>45</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8" t="s">
+      <c r="E47" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" customHeight="1" spans="1:5">
+      <c r="A48" s="9">
+        <v>47</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D48" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E46" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="47" ht="386" customHeight="1" spans="1:5">
-      <c r="A47" s="8">
-        <v>46</v>
-      </c>
-      <c r="B47" s="8" t="s">
+      <c r="E48" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" ht="85" customHeight="1" spans="1:5">
+      <c r="A49" s="9">
+        <v>48</v>
+      </c>
+      <c r="B49" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8" t="s">
+      <c r="C49" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D49" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E47" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48" customHeight="1" spans="1:5">
-      <c r="A48" s="8">
-        <v>47</v>
-      </c>
-      <c r="B48" s="8" t="s">
+      <c r="E49" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" customHeight="1" spans="1:5">
+      <c r="A50" s="9">
+        <v>49</v>
+      </c>
+      <c r="B50" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C48" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D48" s="8" t="s">
+      <c r="C50" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D50" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E48" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="49" ht="85" customHeight="1" spans="1:5">
-      <c r="A49" s="8">
-        <v>48</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D49" s="8" t="s">
+      <c r="E50" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" customHeight="1" spans="1:6">
+      <c r="A51" s="9">
+        <v>50</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D51" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E49" s="8"/>
-    </row>
-    <row r="50" customHeight="1" spans="1:5">
-      <c r="A50" s="8">
-        <v>49</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D50" s="8" t="s">
+      <c r="E51" s="9"/>
+      <c r="F51" s="1"/>
+    </row>
+    <row r="52" ht="137" customHeight="1" spans="1:6">
+      <c r="A52" s="9">
+        <v>51</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D52" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E50" s="8"/>
-    </row>
-    <row r="51" customHeight="1" spans="1:5">
-      <c r="A51" s="8">
-        <v>50</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D51" s="8" t="s">
+      <c r="E52" s="9"/>
+      <c r="F52" s="1"/>
+    </row>
+    <row r="53" ht="286" customHeight="1" spans="1:5">
+      <c r="A53" s="9">
+        <v>53</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E51" s="8"/>
-    </row>
-    <row r="52" ht="137" customHeight="1" spans="1:5">
-      <c r="A52" s="8">
-        <v>51</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D52" s="8" t="s">
+      <c r="E53" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" customHeight="1" spans="1:5">
+      <c r="A54" s="9">
+        <v>54</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E52" s="8"/>
-    </row>
-    <row r="53" ht="286" customHeight="1" spans="1:5">
-      <c r="A53" s="8">
-        <v>53</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8" t="s">
+      <c r="E54" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="55" customHeight="1" spans="1:5">
+      <c r="A55" s="9">
+        <v>55</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D55" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E53" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="54" customHeight="1" spans="1:5">
-      <c r="A54" s="8">
-        <v>54</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8" t="s">
+      <c r="E55" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="56" ht="70" customHeight="1" spans="1:5">
+      <c r="A56" s="9">
+        <v>56</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D56" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E54" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="55" customHeight="1" spans="1:5">
-      <c r="A55" s="8">
-        <v>55</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D55" s="8" t="s">
+      <c r="E56" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" ht="56" customHeight="1" spans="1:5">
+      <c r="A57" s="9">
+        <v>57</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D57" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E55" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="56" ht="70" customHeight="1" spans="1:5">
-      <c r="A56" s="8">
-        <v>56</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E56" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="57" ht="56" customHeight="1" spans="1:5">
-      <c r="A57" s="8">
-        <v>57</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C57" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E57" s="8"/>
+      <c r="E57" s="9" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="58" customHeight="1" spans="1:5">
-      <c r="A58" s="8"/>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
     </row>
     <row r="59" customHeight="1" spans="1:5">
-      <c r="A59" s="8"/>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
+      <c r="A59" s="9"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
     </row>
     <row r="60" customHeight="1" spans="1:5">
-      <c r="A60" s="8"/>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
+      <c r="A60" s="9"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
     </row>
     <row r="61" customHeight="1" spans="1:5">
-      <c r="A61" s="8"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
+      <c r="A61" s="9"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
     </row>
     <row r="62" customHeight="1" spans="1:5">
-      <c r="A62" s="8"/>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
+      <c r="A62" s="9"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
     </row>
     <row r="63" customHeight="1" spans="1:5">
-      <c r="A63" s="8"/>
-      <c r="B63" s="8"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
+      <c r="A63" s="9"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
     </row>
     <row r="64" customHeight="1" spans="1:5">
-      <c r="A64" s="8"/>
-      <c r="B64" s="8"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
+      <c r="A64" s="9"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
     </row>
     <row r="65" customHeight="1" spans="1:5">
-      <c r="A65" s="8"/>
-      <c r="B65" s="8"/>
-      <c r="C65" s="8"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
+      <c r="A65" s="9"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
     </row>
     <row r="66" customHeight="1" spans="1:5">
-      <c r="A66" s="8"/>
-      <c r="B66" s="8"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
+      <c r="A66" s="9"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
     </row>
     <row r="67" customHeight="1" spans="1:5">
-      <c r="A67" s="8"/>
-      <c r="B67" s="8"/>
-      <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="8"/>
+      <c r="A67" s="9"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
     </row>
     <row r="68" customHeight="1" spans="1:5">
-      <c r="A68" s="8"/>
-      <c r="B68" s="8"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="8"/>
+      <c r="A68" s="9"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2988,8 +3015,8 @@
   <sheetPr/>
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="36" customHeight="1" outlineLevelCol="4"/>
@@ -3001,484 +3028,486 @@
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:5">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:5">
-      <c r="A2" s="8">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="8" t="s">
-        <v>74</v>
+      <c r="B2" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="9" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:5">
-      <c r="A3" s="8">
+      <c r="A3" s="9">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="C3" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="4" customHeight="1" spans="1:5">
-      <c r="A4" s="8">
+      <c r="A4" s="9">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" customHeight="1" spans="1:5">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" ht="56" customHeight="1" spans="1:5">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" s="6" customFormat="1" customHeight="1" spans="1:5">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" customHeight="1" spans="1:5">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" customHeight="1" spans="1:5">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" customHeight="1" spans="1:5">
-      <c r="A5" s="8">
-        <v>4</v>
-      </c>
-      <c r="B5" s="8" t="s">
+      <c r="C9" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" ht="62" customHeight="1" spans="1:5">
+      <c r="A10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" ht="56" customHeight="1" spans="1:5">
-      <c r="A6" s="8">
-        <v>5</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="C10" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" customHeight="1" spans="1:5">
+      <c r="A11" s="9">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" s="5" customFormat="1" customHeight="1" spans="1:5">
-      <c r="A7" s="8">
-        <v>6</v>
-      </c>
-      <c r="B7" s="8" t="s">
+      <c r="D11" s="11"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" customHeight="1" spans="1:5">
+      <c r="A12" s="9">
         <v>11</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" customHeight="1" spans="1:5">
-      <c r="A8" s="8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" customHeight="1" spans="1:5">
-      <c r="A9" s="8">
-        <v>8</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" ht="62" customHeight="1" spans="1:5">
-      <c r="A10" s="8">
-        <v>9</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" customHeight="1" spans="1:5">
-      <c r="A11" s="8">
-        <v>10</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" customHeight="1" spans="1:5">
-      <c r="A12" s="8">
-        <v>11</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="B12" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" customHeight="1" spans="1:5">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" customHeight="1" spans="1:5">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" customHeight="1" spans="1:5">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" customHeight="1" spans="1:5">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="8"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" customHeight="1" spans="1:5">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" customHeight="1" spans="1:5">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
     </row>
     <row r="19" customHeight="1" spans="1:5">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="8"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="9"/>
     </row>
     <row r="20" customHeight="1" spans="1:5">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" customHeight="1" spans="1:5">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" s="6" customFormat="1" customHeight="1" spans="1:5">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" s="7" customFormat="1" customHeight="1" spans="1:5">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
     </row>
     <row r="23" customHeight="1" spans="1:5">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:5">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" s="3" customFormat="1" customHeight="1" spans="1:5">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
     </row>
     <row r="25" customHeight="1" spans="1:5">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:5">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-    </row>
-    <row r="27" s="5" customFormat="1" customHeight="1" spans="1:5">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-    </row>
-    <row r="28" s="1" customFormat="1" customHeight="1" spans="1:5">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+    </row>
+    <row r="26" s="3" customFormat="1" customHeight="1" spans="1:5">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+    </row>
+    <row r="27" s="6" customFormat="1" customHeight="1" spans="1:5">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+    </row>
+    <row r="28" s="3" customFormat="1" customHeight="1" spans="1:5">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
     </row>
     <row r="29" customHeight="1" spans="1:5">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
     </row>
     <row r="30" customHeight="1" spans="1:5">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
     </row>
     <row r="31" customHeight="1" spans="1:5">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
     </row>
     <row r="32" customHeight="1" spans="1:5">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
     </row>
     <row r="33" customHeight="1" spans="1:5">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
     </row>
     <row r="34" customHeight="1" spans="1:5">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
     </row>
     <row r="35" customHeight="1" spans="1:5">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
     </row>
     <row r="36" customHeight="1" spans="1:5">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
     </row>
     <row r="37" customHeight="1" spans="1:5">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
     </row>
     <row r="38" customHeight="1" spans="1:5">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
     </row>
     <row r="39" customHeight="1" spans="1:5">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
     </row>
     <row r="40" customHeight="1" spans="1:5">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
     </row>
     <row r="41" customHeight="1" spans="1:5">
-      <c r="A41" s="8">
+      <c r="A41" s="9">
         <v>40</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
     </row>
     <row r="42" customHeight="1" spans="1:5">
-      <c r="A42" s="8">
+      <c r="A42" s="9">
         <v>41</v>
       </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
     </row>
     <row r="43" customHeight="1" spans="1:5">
-      <c r="A43" s="8">
+      <c r="A43" s="9">
         <v>42</v>
       </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
     </row>
     <row r="44" customHeight="1" spans="1:5">
-      <c r="A44" s="8">
+      <c r="A44" s="9">
         <v>43</v>
       </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
     </row>
     <row r="45" customHeight="1" spans="1:5">
-      <c r="A45" s="8">
+      <c r="A45" s="9">
         <v>44</v>
       </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
     </row>
     <row r="46" customHeight="1" spans="1:5">
-      <c r="A46" s="8">
+      <c r="A46" s="9">
         <v>45</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
     </row>
     <row r="47" customHeight="1" spans="1:5">
-      <c r="A47" s="8">
+      <c r="A47" s="9">
         <v>46</v>
       </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
     </row>
     <row r="48" customHeight="1" spans="1:5">
-      <c r="A48" s="8">
+      <c r="A48" s="9">
         <v>47</v>
       </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
     </row>
     <row r="49" customHeight="1" spans="1:5">
-      <c r="A49" s="8">
+      <c r="A49" s="9">
         <v>48</v>
       </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
     </row>
     <row r="50" customHeight="1" spans="1:5">
-      <c r="A50" s="8">
+      <c r="A50" s="9">
         <v>49</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
     </row>
     <row r="51" customHeight="1" spans="1:5">
-      <c r="A51" s="8">
+      <c r="A51" s="9">
         <v>50</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
     </row>
     <row r="52" customHeight="1" spans="1:5">
-      <c r="A52" s="8">
+      <c r="A52" s="9">
         <v>51</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
     </row>
     <row r="53" customHeight="1" spans="1:5">
-      <c r="A53" s="8">
+      <c r="A53" s="9">
         <v>52</v>
       </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
     </row>
     <row r="54" customHeight="1" spans="1:5">
-      <c r="A54" s="8">
+      <c r="A54" s="9">
         <v>53</v>
       </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3507,223 +3536,200 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="D1:H32"/>
+  <dimension ref="D1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" outlineLevelCol="4"/>
   <cols>
     <col min="4" max="4" width="54.75" customWidth="1"/>
-    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="5" max="5" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:6">
+    <row r="1" spans="4:5">
       <c r="D1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+        <v>85</v>
+      </c>
+      <c r="E1" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="4" spans="4:5">
       <c r="D4" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="4:5">
       <c r="D5" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="4:5">
       <c r="D6" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="4:5">
       <c r="D7" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="4:7">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5">
       <c r="D8" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="4:8">
-      <c r="D9" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E9" s="1" t="s">
+    </row>
+    <row r="9" spans="4:5">
+      <c r="D9" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="4:8">
-      <c r="D10" s="1" t="s">
+      <c r="E9" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E10" s="1" t="s">
+    </row>
+    <row r="10" spans="4:5">
+      <c r="D10" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="4:8">
-      <c r="D11" s="1" t="s">
+      <c r="E10" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E11" s="1" t="s">
+    </row>
+    <row r="11" spans="4:5">
+      <c r="D11" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="14" spans="4:6">
+      <c r="E11" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="4:5">
       <c r="D14" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="4:7">
-      <c r="D15" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E15" s="1" t="s">
+    </row>
+    <row r="15" spans="4:5">
+      <c r="D15" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="4:7">
-      <c r="D16" s="1" t="s">
+      <c r="E15" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E16" s="1" t="s">
+    </row>
+    <row r="16" spans="4:5">
+      <c r="D16" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="4:7">
-      <c r="D17" s="1" t="s">
+      <c r="E16" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="E17" s="1" t="s">
+    </row>
+    <row r="17" spans="4:5">
+      <c r="D17" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="20" spans="4:7">
+      <c r="E17" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5">
       <c r="D20" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="4:6">
-      <c r="D21" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E21" s="1" t="s">
+    </row>
+    <row r="21" spans="4:5">
+      <c r="D21" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="4:6">
-      <c r="D22" s="1" t="s">
+      <c r="E21" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E22" s="1" t="s">
+    </row>
+    <row r="22" spans="4:5">
+      <c r="D22" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" ht="19.5" spans="4:6">
-      <c r="D23" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="E23" s="1" t="s">
+    </row>
+    <row r="23" ht="19.5" spans="4:5">
+      <c r="D23" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="4:6">
-      <c r="D24" s="1" t="s">
+      <c r="E23" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E24" s="1" t="s">
+    </row>
+    <row r="24" spans="4:5">
+      <c r="D24" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F24" s="1"/>
+      <c r="E24" s="3" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="27" spans="4:5">
       <c r="D27" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" ht="37.5" spans="4:5">
-      <c r="D28" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="E28" s="4" t="s">
+      <c r="D28" s="5" t="s">
         <v>144</v>
       </c>
+      <c r="E28" s="5" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="29" ht="37.5" spans="4:5">
-      <c r="D29" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="E29" s="4" t="s">
+      <c r="D29" s="5" t="s">
         <v>146</v>
       </c>
+      <c r="E29" s="5" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="30" ht="37.5" spans="4:5">
-      <c r="D30" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="E30" s="4" t="s">
+      <c r="D30" s="5" t="s">
         <v>148</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="4:5">
       <c r="D32" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
file upload by HYP
</commit_message>
<xml_diff>
--- a/残作業リスト.xlsx
+++ b/残作業リスト.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="152">
   <si>
     <t>No.</t>
   </si>
@@ -579,9 +579,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="_-&quot;\&quot;* #,##0_-\ ;\-&quot;\&quot;* #,##0_-\ ;_-&quot;\&quot;* &quot;-&quot;??_-\ ;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;\&quot;* #,##0.00_-\ ;\-&quot;\&quot;* #,##0.00_-\ ;_-&quot;\&quot;* &quot;-&quot;??_-\ ;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_-&quot;\&quot;* #,##0.00_-\ ;\-&quot;\&quot;* #,##0.00_-\ ;_-&quot;\&quot;* &quot;-&quot;??_-\ ;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_-&quot;\&quot;* #,##0_-\ ;\-&quot;\&quot;* #,##0_-\ ;_-&quot;\&quot;* &quot;-&quot;??_-\ ;_-@_-"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -614,9 +614,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="游ゴシック"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="游ゴシック"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="游ゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -629,6 +643,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="游ゴシック"/>
@@ -636,8 +651,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="游ゴシック"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="游ゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -651,17 +675,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="游ゴシック"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFF0000"/>
       <name val="游ゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -669,13 +684,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="游ゴシック"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="游ゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -696,9 +704,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="3"/>
+      <name val="游ゴシック"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="游ゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -717,22 +733,6 @@
       <color theme="3"/>
       <name val="游ゴシック"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="游ゴシック"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="游ゴシック"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -822,7 +822,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -834,19 +906,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -858,145 +990,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1038,17 +1038,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1060,6 +1049,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1079,6 +1079,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1090,15 +1099,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1143,145 +1143,145 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3096,7 +3096,9 @@
         <v>97</v>
       </c>
       <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="E5" s="9" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="6" ht="56" customHeight="1" spans="1:5">
       <c r="A6" s="9">
@@ -3109,7 +3111,9 @@
         <v>99</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="E6" s="9" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="7" s="6" customFormat="1" customHeight="1" spans="1:5">
       <c r="A7" s="9">
@@ -3122,7 +3126,9 @@
         <v>100</v>
       </c>
       <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="E7" s="9" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="8" customHeight="1" spans="1:5">
       <c r="A8" s="9">
@@ -3135,7 +3141,9 @@
         <v>102</v>
       </c>
       <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="E8" s="9" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="9" customHeight="1" spans="1:5">
       <c r="A9" s="9">
@@ -3174,7 +3182,9 @@
         <v>97</v>
       </c>
       <c r="D11" s="11"/>
-      <c r="E11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="12" customHeight="1" spans="1:5">
       <c r="A12" s="9">

</xml_diff>

<commit_message>
footer ph no added and recruit form mail setting repair by HYP
</commit_message>
<xml_diff>
--- a/残作業リスト.xlsx
+++ b/残作業リスト.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="152">
   <si>
     <t>No.</t>
   </si>
@@ -579,8 +579,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_-&quot;\&quot;* #,##0.00_-\ ;\-&quot;\&quot;* #,##0.00_-\ ;_-&quot;\&quot;* &quot;-&quot;??_-\ ;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_-&quot;\&quot;* #,##0_-\ ;\-&quot;\&quot;* #,##0_-\ ;_-&quot;\&quot;* &quot;-&quot;??_-\ ;_-@_-"/>
   </numFmts>
   <fonts count="25">
@@ -607,6 +607,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="游ゴシック"/>
@@ -615,14 +623,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="游ゴシック"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="游ゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -635,8 +636,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="游ゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -656,17 +658,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF0000FF"/>
       <name val="游ゴシック"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
       <name val="游ゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -682,7 +683,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="游ゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -696,7 +697,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="游ゴシック"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -719,14 +720,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="游ゴシック"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="游ゴシック"/>
@@ -742,6 +735,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="游ゴシック"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -752,9 +752,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="游ゴシック"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -822,7 +822,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -834,31 +906,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -870,7 +930,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -882,43 +960,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -930,73 +996,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1040,9 +1040,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1077,21 +1094,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1103,6 +1105,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1124,17 +1135,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1143,7 +1143,7 @@
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1152,136 +1152,136 @@
     <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3016,7 +3016,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="$A10:$XFD10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="36" customHeight="1" outlineLevelCol="4"/>
@@ -3195,7 +3195,9 @@
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
+      <c r="E12" s="9" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="13" customHeight="1" spans="1:5">
       <c r="A13" s="9"/>

</xml_diff>